<commit_message>
Wolf Added to Scene, Animations Fixed, Game Speed Increase over time added
</commit_message>
<xml_diff>
--- a/Documents/Fabled_Carnage_Geschwindigkeit.xlsx
+++ b/Documents/Fabled_Carnage_Geschwindigkeit.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Descus\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25905CB2-02CC-46F7-A670-9CD4036F1C03}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28455" yWindow="345" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28455" yWindow="345" windowWidth="20910" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -65,19 +59,19 @@
     <t>/ 60)</t>
   </si>
   <si>
-    <t xml:space="preserve"> / 60)</t>
+    <t xml:space="preserve"> / 90)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,8 +124,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -151,9 +145,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,9 +185,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,26 +220,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,26 +255,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -470,11 +430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:LL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:LL2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5065,7 +5025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5077,7 +5037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>